<commit_message>
BOM Expansion with three pos: temperature sensor, heating cable and relay
</commit_message>
<xml_diff>
--- a/bill of matirials.xlsx
+++ b/bill of matirials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicks\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2345b08f47418127/Projekte/Terralogia.git/Terralogia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF926B0-D650-49F8-9F13-79B3B7129624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{FFF926B0-D650-49F8-9F13-79B3B7129624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4083F4B2-CE99-4024-AD31-7DC85BD16153}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electric Hardware" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Pos</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>Preis per Einheit</t>
+  </si>
+  <si>
+    <t>Temperatur Sensor</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>Heizkabel</t>
   </si>
 </sst>
 </file>
@@ -192,8 +201,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B0F07CF0-7A5E-4B70-B479-EEEF4282E19D}" name="Tabelle2" displayName="Tabelle2" ref="C5:G14" totalsRowShown="0">
-  <autoFilter ref="C5:G14" xr:uid="{B0F07CF0-7A5E-4B70-B479-EEEF4282E19D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B0F07CF0-7A5E-4B70-B479-EEEF4282E19D}" name="Tabelle2" displayName="Tabelle2" ref="C5:G17" totalsRowShown="0">
+  <autoFilter ref="C5:G17" xr:uid="{B0F07CF0-7A5E-4B70-B479-EEEF4282E19D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BF0D56A8-4590-4122-86AE-35C7241E2006}" name="Pos" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{8B278A4B-AFF8-46F3-91E7-0B3D9461C472}" name="Bezeichner"/>
@@ -485,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C5:G14"/>
+  <dimension ref="C5:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,6 +647,39 @@
       </c>
       <c r="G14" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -764,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231290C6-FF6F-4F35-87EF-999B72D02B34}">
   <dimension ref="C4:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>